<commit_message>
fix data set errors
</commit_message>
<xml_diff>
--- a/StudentResults.xlsx
+++ b/StudentResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtapi\Documents\JP\team-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F286CD55-48BA-4411-A266-A135C556937F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C457436-5559-4EBC-B604-66E13CE6BBCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="5244" windowWidth="17280" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="804" windowWidth="17280" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student Results" sheetId="1" r:id="rId1"/>
@@ -362,8 +362,8 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>